<commit_message>
Updated reveal.js. Finished lesson 2
</commit_message>
<xml_diff>
--- a/spliced_files.xlsx
+++ b/spliced_files.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Raksit/Documents/Documents/Ryukyu Metadata/sakishima/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{939F5496-8E66-EE4D-A443-8832A3AABFC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C86CFD-BA40-EB43-B26F-F3AAA3EB7278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-31800" yWindow="480" windowWidth="28800" windowHeight="17500" xr2:uid="{C0B25C98-D615-ED44-8938-EEEE559432F2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>lesson</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>aaiureegusiaranuureepytuju.wav</t>
+  </si>
+  <si>
+    <t>uree-unupytu.wav</t>
+  </si>
+  <si>
+    <t>unupytu.wav</t>
   </si>
 </sst>
 </file>
@@ -430,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47F9E6EE-D830-E846-A989-3DFEFF300BDA}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -550,7 +556,24 @@
         <v>14</v>
       </c>
     </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>